<commit_message>
Add polynomial regression analysis with R comparison to Paises page
</commit_message>
<xml_diff>
--- a/Desembolsos_Acum_Max.xlsx
+++ b/Desembolsos_Acum_Max.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Downloads\desembolsos-main\desembolsos-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07A7419-F8E8-4698-A6EE-D5CA25746C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58524CAD-1CA9-478E-8D57-056FF5BF1734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-1275" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$478</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -683,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H478"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A451" workbookViewId="0">
+      <selection activeCell="D466" sqref="D466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9716,7 +9719,7 @@
         <v>97</v>
       </c>
       <c r="B348">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C348">
         <v>0.28571428571428598</v>
@@ -9742,7 +9745,7 @@
         <v>97</v>
       </c>
       <c r="B349">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C349">
         <v>1</v>
@@ -13118,6 +13121,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H478" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>